<commit_message>
chore: updated version number
</commit_message>
<xml_diff>
--- a/runwaysdk-test/test.xlsx
+++ b/runwaysdk-test/test.xlsx
@@ -71,9 +71,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="18.19140625" customWidth="true"/>
-    <col min="2" max="2" width="15.63671875" customWidth="true"/>
-    <col min="3" max="3" width="15.734375" customWidth="true"/>
+    <col min="1" max="1" width="16.64453125" customWidth="true"/>
+    <col min="2" max="2" width="14.421875" customWidth="true"/>
+    <col min="3" max="3" width="14.57421875" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1" hidden="true">

</xml_diff>